<commit_message>
Update test excel and remove unnecessary awaits
</commit_message>
<xml_diff>
--- a/end-to-end-tests/excel-importer.xlsx
+++ b/end-to-end-tests/excel-importer.xlsx
@@ -265,7 +265,7 @@
     <t xml:space="preserve">Test Ali Excel</t>
   </si>
   <si>
-    <t xml:space="preserve">_1B_ONHERROEPELIJK_MET_UITWERKING_NODIG</t>
+    <t xml:space="preserve">Afgerond</t>
   </si>
 </sst>
 </file>
@@ -811,7 +811,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="189">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1565,10 +1565,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="44" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1675,8 +1671,8 @@
   </sheetPr>
   <dimension ref="B1:GE44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3133,7 +3129,7 @@
       <c r="GD5" s="136"/>
       <c r="GE5" s="137"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="138" t="n">
         <v>1211122121</v>
       </c>
@@ -9576,8 +9572,6 @@
       <c r="AK40" s="0"/>
       <c r="AL40" s="0"/>
       <c r="AM40" s="0"/>
-      <c r="AN40" s="189"/>
-      <c r="AO40" s="189"/>
       <c r="AP40" s="0"/>
       <c r="AQ40" s="0"/>
       <c r="AR40" s="0"/>
@@ -9764,8 +9758,6 @@
       <c r="AK41" s="0"/>
       <c r="AL41" s="0"/>
       <c r="AM41" s="0"/>
-      <c r="AN41" s="189"/>
-      <c r="AO41" s="189"/>
       <c r="AP41" s="0"/>
       <c r="AQ41" s="0"/>
       <c r="AR41" s="0"/>
@@ -9952,8 +9944,6 @@
       <c r="AK42" s="0"/>
       <c r="AL42" s="0"/>
       <c r="AM42" s="0"/>
-      <c r="AN42" s="189"/>
-      <c r="AO42" s="189"/>
       <c r="AP42" s="0"/>
       <c r="AQ42" s="0"/>
       <c r="AR42" s="0"/>
@@ -10140,8 +10130,6 @@
       <c r="AK43" s="0"/>
       <c r="AL43" s="0"/>
       <c r="AM43" s="0"/>
-      <c r="AN43" s="189"/>
-      <c r="AO43" s="189"/>
       <c r="AP43" s="0"/>
       <c r="AQ43" s="0"/>
       <c r="AR43" s="0"/>
@@ -10328,8 +10316,6 @@
       <c r="AK44" s="0"/>
       <c r="AL44" s="0"/>
       <c r="AM44" s="0"/>
-      <c r="AN44" s="189"/>
-      <c r="AO44" s="189"/>
       <c r="AP44" s="0"/>
       <c r="AQ44" s="0"/>
       <c r="AR44" s="0"/>

</xml_diff>